<commit_message>
SI and heating demands
</commit_message>
<xml_diff>
--- a/model_material/U_values/U-Values_final.xlsx
+++ b/model_material/U_values/U-Values_final.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11010" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="7470" windowHeight="8595" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="all_u_values" sheetId="1" r:id="rId1"/>
@@ -2293,8 +2293,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AJ37"/>
   <sheetViews>
-    <sheetView topLeftCell="O1" workbookViewId="0">
-      <selection activeCell="T4" sqref="T4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3974,8 +3974,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D7" workbookViewId="0">
-      <selection activeCell="T9" sqref="T9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>